<commit_message>
Improvements and adding questions
</commit_message>
<xml_diff>
--- a/output_single_question_pivoted.xlsx
+++ b/output_single_question_pivoted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter**: CGIAR Region.
+          <t>**Parameter**: CGIAR Region.
 **Description:** The CGIAR geographic region where the study took place, based on the following categories. If the study took place/focused on a single country, then choose the region where that country would be located. If it spanned several countries that end up belonging to more than one of the regions below, then reply instead with "Multiple". The categories are:
 - (1) ESA: "East and Southern Africa"
 - (2) WCA: "West and Central Africa"
@@ -454,7 +454,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Category for Natural Resource Management.
+          <t>**Parameter:** Category for Natural Resource Management.
 **Description:** The study would identify the practices that the CGIAR center is studying. These practices regard in general the stewardship of ecosystems, biodiversity, soil health, water systems, and climate resilience to ensure sustainable food production. You have to go through the document/content and identify the main practices the study identified, is concerned about; or to which its content/impact is related. You should then assign one of the categories below and return that as your answer. Some categories are general, like "Crop management" while others are more specific, like "Crop management - agroforestry." Assign first the general category to the Natural Resource Management practices identified in the study and then do another pass to see if there is enough information to apply instead one of the more specific labels/categories. The categories are:
 - Aquaculture
 - Crop management
@@ -491,7 +491,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Category of Study.
+          <t xml:space="preserve">**Parameter:** Category of Study.
 **Description:** The category of the study; based on what it is about. Read through the content and then assign accordingly 1 of the following 5 categories:
 - (1) Ex post impact study/impact assesment;
 - (2) Outcome studies;
@@ -503,14 +503,42 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Country of Study.
+          <t>**Parameter:** Contributing Initiatives or centers.
+**Description:** CGIAR is associated with multiple Initiatives and Centers. You need to extract the names of the ones mentioned in the text, if any.
+**Output Format:** Your response should be a string with values separated by commas. For example "CIMMYT, AgriLac Resiliente, ICARDA".</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Country of Study.
 **Description:** The name of the country where the study/observations took place.
 **Output Format:** Reply with the name of the country, e.g. "Spain". If the study took place in more than one country, then reply "Multiple".</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Name; Unit/Metric; and Value for Reported Indicator of Impact.
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Crops.
+**Description:** Create a list of any of the crops mentioned in the text.
+**Output Format:** Your response should be a string with values separated by commas.</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Keywords.
+**Description:** Create a list of the top 5 most relevant keywords from this article.
+**Output Format:** Your response should be a string with values separated by commas.</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Link or DOI.
+**Description:** Extract the DOI or URL that references to this article in its content.
+**Output Format:** Your response should be a string with the URL.</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Name; Unit/Metric; and Value for Reported Indicator of Impact.
 **Description:** Some studies use/report an Indicator of Impact to assess the impact/outcome of CGIAR contributions, as a way to measure it. Go through the content and identify the Indicator of Impact used, and then identify what unit/metric is used to measure it, and then identify its value. For example:
 - "Increase in farmable land; hectares; 3"
 The unit/metric and its associated value will be whatever is used to measure the Indicator.
@@ -518,25 +546,25 @@
 **Output Format:** When an Indicator of Impact is reported and identified, return the name, unit/metric, and  value of the most relevant one like this "Name; Unit/Metric; Value". For example "Increase in gender engagement; Number of women; 1300" or "Increase in profits from selling crops; thousands of USD; 12", etc. If no Indicator is reported, return instead "Not reported; NA; NA"</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Period Analyzed.
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Period Analyzed.
 **Description:** The period of time covered by the study; whether it is e.g. the period of time during which a particular approach was undertaken or the span of time during which some results are viewed/or observations post-factum are made. As they can be for example, an approach undertaken during 2 years, or a report reviewing progress across X years after the approach was complete.
 **Output Format:** Your reply must specify the start and end dates as four digit years separated by a dash, for example "1994-2002".</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Primary Product Type.
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Primary Product Type.
 **Description:** The primary production of the agrifood system that the CGIAR center is studying. Identify the type of the primary product and then categorize it based on the vocabulary used in AGROVOC. For example:
 - (1) Cultivation of crops (e.g. cereals, legumes, fruits, and vegetables)
 - (2) Rearing of livestock (e.g. cattle, poultry, fish, other animal species) for food, feed, fiber, and bioenergy
 **Output Format:** Your response should be a string with the categorization for the primary product type, identifying the product and where applicable, its purpose. For example "Cultivation of crops (legumes)" or "Rearing of livesock (cattle) for food". Use your judgement and AGROVOC vocabulary for the response wording.</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Primary and Secondary CGIAR Impact Area(s).
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Primary and Secondary CGIAR Impact Area(s).
 **Description:** The CGIAR Impact Area(s) the study addresses. The study should have/target at least one Impact Area. If the study addresses more than one Impact Area, identify all that would apply and rank them internally based on the most fitting to the document based on the descriptions below.
 - (1) "Nutrition, health and food security": "Enable affordable, healthy diets for the 3 billion people who currently lack access to safe and nutritious food. Decrease cases of foodborne illness and zoonotic diseases by one-third."
 - (2) "Poverty reduction, livelihoods and jobs": "Lift at least 500 million people living in rural areas above the extreme poverty line of US $1.90 per day. Reduce by at least half the proportion of people of all ages living in poverty in all its dimensions."
@@ -546,16 +574,30 @@
 **Output Format:** If the study focuses only on one main Impact Area, then return the name of the Impact Area (from those above), without the description in this format: "Main Area Name; No Secondary Impact Area(s)". For example: "Climate adaptation and mitigation; No Secondary Impact Area(s)". If targeting multiple Impact Areas, then your response will be the name of the applicable Impact Areas based on your internal ranking, separated by semicolors, starting from the most relevant/targeted and then going down from there. For example, if it targets two, it could be something like this: "Environmental health and biodiversity; Climate adaptation and mitigation".</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Study Theme.
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Study Theme.
 **Description:** The main topic/theme of the study; which is the attribution/contribution of CGIAR interventions/policies/innovations by a CGIAR center. There are no predefined categories for this parameter.
 **Output Format:** Your answer should be in the format of a short title that outlines the theme.</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>After having gone through the PDF/document above, extract the specific parameter outlined below based on the contextual description/information accompanying it, and always replying strictly as outlined in the Output Format below.**Parameter:** Year of Report.
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Summary.
+**Description:** Create a summary of the text provided.
+**Output Format:** Your answer should be in the format of 1 or 2 paragraphs, that summarizes the text.</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Title.
+**Description:** The title of the document.
+**Output Format:** Your answer should be in the format of a short title, directly extracted from the text</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>**Parameter:** Year of Report.
 **Description:** The date on which the study/document was published.
 **Output Format:** Output a single 4 digit year. E.g. "2002"</t>
         </is>
@@ -584,35 +626,66 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Alliance of Bioversity International and CIAT, East West Seed Knowledge Transfer, NARO, AVRDC</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Uganda</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>vegetables</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>vegetable production, smallholder systems, climate change adaptation, Uganda, livelihood improvement</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>&lt;Not Defined&gt;</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>2020-2020</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Cultivation of crops (vegetables)</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>"Climate adaptation and mitigation; Environmental health and biodiversity; Poverty reduction, livelihoods and jobs"</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Introduction of Vegetable Production for Livelihood Improvement and Climate Adaptation</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>"Climate adaptation and mitigation; Environmental health and biodiversity"</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Introduction of vegetable production in smallholder systems for livelihood improvement and climate change adaptation</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>The document reports on a study titled "Introduction of vegetable production in smallholder systems: a promising option for livelihood improvement and climate change adaptation," completed in 2020. This initiative was coordinated by East West Seed Knowledge Transfer, the Alliance of Bioversity International and CIAT, the World Vegetable Centre, and Uganda's National Agricultural Research Organisation. It aimed to introduce and test a variety of commercial and traditional vegetables in Uganda's Hoima district to help resource-poor farmers adapt to climate change by increasing the availability and diversity of climate-smart varieties. The project also sought to enhance farmers' capacity to utilize vegetable crop diversity for various livelihood purposes, yielding positive results.
+The study aligns with the CGIAR Strategic Results Framework, contributing to diversified enterprise opportunities, increased resilience of agro-ecosystems and communities, and enhanced adaptive capacity to climate risks. It is linked to the SRF 2022/2030 target of increasing the number of farm households adopting improved varieties, breeds, or trees. The pilot project's success in Hoima district suggests potential for replication in other districts, provided farmers receive motivation and initial technical support. The geographic scope of the study is national, focusing on Uganda.</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Introduction of vegetable production in smallholder systems: a promising option for livelihood improvement and climate change adaptation</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -641,35 +714,65 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>CIMMYT, EIAR</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Ethiopia</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Durum wheat, wheat</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Wheat, Seed Scaling, Ethiopia, Genetic Gains, USAID</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>&lt;Not Defined&gt;</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>2015-2019</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>Lessons Learnt from the Wheat Seed Scaling Project in Ethiopia</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>The document titled "Reporting 2021 Evidences" focuses on a study identified as #3962, which involves projects aimed at enhancing wheat production in Ethiopia. The contributing projects include building rust screening capacity for durum wheat and delivering genetic gains in wheat. The study, commissioned by USAID, assesses the impact of the Wheat Seed Scaling Project conducted from 2015 to 2019. It highlights lessons learned and recommendations regarding the fast-track variety release process and the challenges in establishing a sustainable durum wheat value chain for pasta production. The study aligns with CGIAR's strategic goals, particularly in increasing the adoption of improved agricultural materials and meeting dietary energy requirements. The geographic focus is national, specifically targeting Ethiopia. The report was generated on August 19, 2022.</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Lessons Learnt from the Wheat Seed Scaling Project 2015-2019</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -698,35 +801,66 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>BBSRC, MAIZE, CISANET</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Malawi</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Maize</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Conservation Agriculture, Soil Hydraulic Conductivity, Water Retention, Maize-based Systems, Malawi</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>&lt;Not Defined&gt;</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>2010-2022</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>"Environmental health and biodiversity; Climate adaptation and mitigation"</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Conservation Agriculture's Impact on Soil Hydraulic Properties in Malawi</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Conservation Agriculture's Impact on Soil Hydraulic Properties and Water Retention in Malawi</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>The document reports on a study titled "Long term (10–12 years) maize-based Conservation Agriculture's impact on soil hydraulic conductivity &amp; water retention (Malawi)," which was completed in 2020. The study, commissioned by BBSRC, MAIZE, and CISANET, evaluates the impact of conservation agriculture (CA) on soil properties in Malawi. It highlights that CA systems significantly improve soil hydraulic properties and structure, although no significant increase in soil organic matter was observed, suggesting a need for better crop residue management. The study underscores CA's potential to enhance water storage and availability during dry spells and recommends future research to assess carbon balance and soil organic matter pathways.
+The study is linked to several projects, including MISST, DeSIRA, and Africa RISING, and aligns with the CGIAR Strategic Results Framework targets for 2022/2030, focusing on improved agronomic practices and increased water and nutrient use efficiency. The geographic scope of the study is both national and regional, specifically targeting Southern Africa and Malawi. The findings contribute to understanding CA's role in sustainable agriculture and its potential benefits for soil and water management in Sub-Saharan Africa.</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Long term (10–12 years) maize-based Conservation Agriculture's impact on soil hydraulic conductivity &amp; water retention (Malawi)</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -755,35 +889,66 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>International Institute of Tropical Agriculture (IITA)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>Kenya</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>maize, groundnut, cereals, oilseeds, spices, tree nuts, milk, meat, dried fruits, legumes</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Aflatoxins, Biological control, Aflasafe KE01, Willingness to Pay (WTP), Contingent Valuation Method (CVM)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/19440049.2020.1817571</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>2014-2014</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>Willingness-to-Pay for Aflasafe KE01 for Aflatoxin Management in Kenya</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>The document discusses a study on the willingness-to-pay (WTP) for Aflasafe KE01, a biological control product designed to manage aflatoxin contamination in maize in Kenya. The study utilized the Contingent Valuation Method (CVM) to assess WTP among 480 farmers across four aflatoxin-prone counties: Makueni, Machakos, Kitui, and Tana River. The mean WTP per kilogram of Aflasafe KE01 ranged from Ksh 113 to 152, compared to a similar product in Nigeria priced at Ksh 130/kg. Factors positively influencing WTP included access to extension services, credit, and awareness of the product. The study highlights the need for increased education and integration of the product into credit schemes to facilitate adoption.
+The research also examined socio-economic characteristics of the households, finding that most farmers were willing to pay for the product, with higher WTP in regions with previous aflatoxin outbreaks. The study suggests that awareness and access to credit are crucial for adoption, and recommends enhancing distribution networks and awareness campaigns to support scaling efforts. The findings provide insights into pricing strategies and policy formulation to expand the market for Aflasafe KE01, emphasizing the importance of addressing the heterogeneous nature of maize farmers in Kenya.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Assessment of willingness-to-pay for Aflasafe KE01, a native biological control product for aflatoxin management in Kenya</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -802,7 +967,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Crop management - improved varieties</t>
+          <t>Crop management - varietal adoption</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -812,35 +977,66 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>ICARDA, CIMMYT</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>Morocco</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Durum wheat, wheat, rice</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>breeding objectives, participatory farmers-weighted selection indices, durum wheat, Morocco, adoption</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.20900/cbgg20200014</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>2014-2015</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Cultivation of crops (cereals)</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>"Cultivation of crops (cereals)"</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>"Poverty reduction, livelihoods and jobs; Climate adaptation and mitigation"</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Participatory Farmers-Weighted Selection Indices to Enhance Durum Cultivar Adoption in Morocco</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Participatory Farmers-Weighted Selection Indices to Enhance Adoption of Durum Cultivars in Morocco</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>The article discusses the challenges and potential solutions for increasing the adoption of new durum wheat cultivars in Morocco. It highlights the misalignment between the breeding objectives of North African breeders and the preferences of Moroccan farmers, which contributes to the low adoption rates of improved cultivars. The study uses participatory farmers-weighted selection (PWS) indices to better align breeders' objectives with farmers' needs. By analyzing data from interviews with wheat breeders and a survey of Moroccan farmers, the study identifies discrepancies in trait preferences, such as yield potential, industrial quality, and household use. The research suggests that using PWS indices could help bridge the gap between breeders and farmers, leading to higher adoption rates of new cultivars. The study also emphasizes the importance of considering farmers' socio-economic contexts and preferences in breeding programs to ensure the development of cultivars that meet their needs.
+The article further explores the performance of 23 ICARDA durum wheat elite lines, revealing that while some cultivars align well with farmers' preferences, others do not. The study concludes that a more systemic approach, incorporating farmers' input through PWS indices, could enhance the effectiveness of breeding programs in developing countries. It also suggests that while participatory variety selection (PVS) has been beneficial, PWS indices offer a more scalable and cost-effective alternative for integrating farmers' preferences into breeding objectives. The research underscores the need for breeders to ensure alignment with farmers' priorities to improve the adoption of new cultivars and address the challenges faced by smallholder farmers in developing regions.</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Participatory Farmers-Weighted Selection (PWS) Indices to Raise Adoption of Durum Cultivars</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -869,35 +1065,65 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>IWMI, Bioversity, CIAT, ICARDA, ICRISAT, IFPRI, World Agroforestry Center, FAO, RUAF, CIFOR, CIP, ILRI, WorldFish</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>crop production, crop health card</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Water, Land, Ecosystems, Sustainable, CGIAR</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://cas.cgiar.org/</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>2017-2019</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals, legumes, fruits, and vegetables)</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Environmental health and biodiversity; Climate adaptation and mitigation</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Water, Land, and Ecosystem Management Innovations in Agricultural Landscapes</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>"Environmental health and biodiversity; Climate adaptation and mitigation"</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Water, Land, and Ecosystem Management Innovations and Investments in Agricultural Landscapes.</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>The CGIAR Research Program on Water, Land and Ecosystems (WLE) is a global initiative aimed at providing evidence-based solutions for sustainable management of water, land, and ecosystems to enhance resilience and reduce risks in agricultural landscapes, particularly in developing countries. The program, led by the International Water Management Institute (IWMI), collaborates with several CGIAR Centers and partners to address critical global challenges through five flagship programs. The review of WLE's work from 2017 to 2019 highlights its achievements in delivering quality science and effectiveness, despite funding constraints. WLE has successfully completed 90% of its milestones, developed 32 innovations, and influenced 20 policies, including contributions to global environmental agreements and Sustainable Development Goals (SDGs). The program's management and governance have fostered collaboration and transparency, although its potential as a global integrator has been limited by funding structures. WLE's experiences in applying integrated systems approaches offer significant opportunities for One CGIAR, particularly in addressing complex global challenges at the interface of livelihoods, ecosystem services, and food and water security. The review recommends showcasing WLE's role as a thought leader, synthesizing program results, and enhancing capacity development and partnership strategies to inform future CGIAR research modalities.</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>CGIAR Research Program 2020 Reviews: Water, Land and Ecosystems (WLE)</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -926,35 +1152,65 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>CIP, RTB, INIAP, Agrocalidad, MAG, FAO, OIRSA, IICA, CAN, INIA, Senasa, McKnight Foundation, Syngenta, Central University of Ecuador, Ekorural, CONPAPA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>Ecuador</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Potato, Cassava, Bananas, Plantains, Sweetpotato, Yams, Minor roots and tubers</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Potato Purple Top, Ecuador, CGIAR, INIAP, Agrocalidad</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>10.4160/9789290605553</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>2012-2020</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>Cultivation of crops (potatoes)</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Poverty reduction, livelihoods and jobs; Environmental health and biodiversity</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>"Poverty reduction, livelihoods and jobs; Nutrition, health and food security; Environmental health and biodiversity"</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
         <is>
           <t>Control of Potato Purple Top in Ecuador: Evaluation of CGIAR Contributions to Policy Outcome Trajectory</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>The document evaluates the contributions of the CGIAR Research Programs on Roots, Tubers, and Bananas (RTB) to the control of potato purple top (PMP) disease in Ecuador. It highlights the establishment of a national-level technical committee to develop a coordinated strategy for PMP control, supported by research and risk assessments from CIP and RTB. The evaluation identifies strategies that contributed to a shift in social norms, capacity building, and a strengthened support base, which are crucial for policy change. Despite progress, challenges remain, such as the need for a clearer understanding of PMP's threat and effective control measures, as well as securing more resources for sustained efforts. The document also notes that gender considerations have not yet been integrated into the PMP control trajectory, although research is underway to address this. Overall, the evaluation underscores the importance of continued research, clearer communication, and regional collaboration to effectively manage PMP in Ecuador.</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Control of potato purple top in Ecuador: Evaluation of CGIAR contributions to a policy outcome trajectory</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -983,35 +1239,65 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>IITA, RTB, A4NH, CIP</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>Rwanda</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>cassava, beans, bananas, maize, rice, wheat, peas, sweetpotatoes, vegetable seeds</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>cassava seed certification, Rwanda, CGIAR, policy outcome trajectory, CBSD</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>10.4160/9789290605638</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>2017-2020</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>Cultivation of crops (cassava)</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs; Gender equality, youth and social inclusion</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Development of a Cassava Seed Certification System in Rwanda</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Poverty reduction, livelihoods and jobs; Nutrition, health and food security; Gender equality, youth and social inclusion</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Development of a Cassava Seed Certification System in Rwanda: Evaluation of CGIAR Contributions to Policy Change</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>The document evaluates the development of a cassava seed certification system in Rwanda, focusing on the contributions of CGIAR, particularly through the International Institute for Tropical Agriculture (IITA) and the CGIAR Research Program on Roots, Tubers, and Bananas (RTB). The study highlights the significant role of IITA/RTB in facilitating the approval of cassava seed standards by the Rwanda Standards Board in 2018, which was achieved in less than a year. This rapid progress was attributed to the strong collaboration between IITA, RAB, and RSB, and the learning from similar processes in Tanzania. The document outlines the strategies used to achieve a shift in social norms, capacity building, and strengthening the support base for the cassava seed system. It also discusses the challenges of making clean planting material available to farmers and the ongoing efforts to develop viable agribusiness models. The study concludes that the cassava seed standards trajectory is likely to be sustained and scaled over the long term, given the momentum and support from various stakeholders and projects.</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Development of a cassava seed certification system in Rwanda: Evaluation of CGIAR contributions to a policy outcome trajectory</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1040,35 +1326,65 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>IITA, CIP, RTB, CIAT, CIRAD</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>Tanzania</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>cassava, potato, sweetpotato, bananas, plantains, yams, minor roots and tubers</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>cassava seed certification, Tanzania, CGIAR, cassava diseases, policy outcome trajectory</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>10.4160/9789290605560</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1930s-2020</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2012-2020</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
         <is>
           <t>Cultivation of crops (cassava)</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Development of a Cassava Seed Certification System in Tanzania</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs; Gender equality, youth and social inclusion</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Development of a Cassava Seed Certification System in Tanzania: Evaluation of CGIAR Contributions to Policy Change</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>The document evaluates the development of a cassava seed certification system in Tanzania, focusing on the contributions of CGIAR, particularly through the International Institute for Tropical Agriculture (IITA) and the CGIAR Research Program on Roots, Tubers and Bananas (RTB). The study highlights the historical context of cassava diseases like cassava mosaic disease (CMD) and cassava brown streak disease (CBSD), which have driven the need for certified disease-resistant planting material. The document outlines the collaborative efforts of IITA, TOSCI, TARI, and MEDA, supported by the Bill and Melinda Gates Foundation, to establish seed certification protocols and regulations, which were signed into law in 2017. The evaluation uses the Policy Windows theory of change to analyze how policy changes occurred, emphasizing the importance of a coalition of stakeholders, capacity building, and market development for cassava. The study concludes that the seed certification trajectory is likely to be sustained due to political support, a strong coalition, and ongoing financial backing, although challenges remain in scaling the system and integrating gender considerations.</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Development of a cassava seed certification system in Tanzania: Evaluation of CGIAR contributions to a policy outcome trajectory</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1097,35 +1413,66 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>CIAT</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>Rwanda</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>cassava, maize, beans, peanuts, Irish potatoes, vegetables</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Gender, climate services, evaluation, Rwanda, agriculture</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>https://ccafs.cgiar.org/donors</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>2016-2020</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Cultivation of crops (cereals and legumes)</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Cultivation of crops (cereals)</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t>"Climate adaptation and mitigation; Gender equality, youth and social inclusion; Poverty reduction, livelihoods and jobs"</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>Rwanda Climate Services for Agriculture: Gender-Sensitive Evaluation of Climate Information Access and Use</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>The working paper "Rwanda Climate Services for Agriculture: Qualitative Evaluation through a Gender Lens" evaluates the Rwanda Climate Services for Agriculture project, which ran from 2016 to 2020. The project aimed to enhance smallholder farmers' resilience to climate variability through interventions like Participatory Integrated Climate Services for Agriculture (PICSA) and Radio Listeners’ Clubs (RLC). The evaluation, conducted in October 2019, focused on gender differences in access to and use of climate information, and the benefits derived from climate-informed decisions. Data was collected through focus group discussions and key informant interviews across Rwanda's provinces, revealing that both women and men primarily accessed weather and climate information through radios and Farmer Promoters. However, women reported using peer networks more, while men used a broader range of channels, including television.
+The study found that project interventions helped narrow the gender gap in the use of climate information, particularly for women, who reported increased use of climate information for farm decision-making. Both women and men perceived benefits such as increased yields, income, and food security from climate-informed decisions, with interventions contributing to these outcomes. The evaluation also noted that women's participation in household decision-making improved due to enhanced climate knowledge and successful application of climate-informed practices. Recommendations include promoting more opportunities for women to participate in interventions, assessing gender-specific decision-making processes, and incorporating women's enhanced voice in agricultural decision-making into project planning. The study highlights the importance of understanding gender dynamics in climate services to ensure equitable access and benefits.</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Rwanda Climate Services for Agriculture: Qualitative Evaluation through a Gender Lens</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1139,50 +1486,80 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>ESA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Crop management - improved varieties</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Outcome studies</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CIMMYT, CIAT, IITA, CIP, IFPRI, HarvestPlus, RTB, A4NH, FARA, AUDA-NEPAD, AUC-DREA, AUC-DSA</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Crop management - improved varieties</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Outcome studies</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Multiple</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>orange fleshed sweetpotato, rice, wheat, maize, beans, cassava, millet</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>biofortification, African Union, CGIAR, policy change, nutrition</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>10.4160/978929060-5522</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>2014-2020</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>Cultivation of crops (roots and tubers)</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>Nutrition, health and food security; Gender equality, youth and social inclusion</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Mainstreaming of Biofortification in the African Union: Evaluation of CGIAR Contributions to Policy Change</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Mainstreaming Biofortification in the African Union: Evaluation of CGIAR Contributions</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>The document evaluates the contributions of CGIAR, particularly the Research Programs on Roots, Tubers and Bananas (RTB) and Agriculture for Nutrition and Health (A4NH), in mainstreaming biofortification within the African Union (AU). It highlights the collaborative efforts of HarvestPlus/A4NH and CIP/RTB in advocating for biofortification as a solution to micronutrient malnutrition, leading to a continental declaration ready to be tabled at an AU Summit. The evaluation uses a policy window theory of change to understand how CGIAR's framing of the problem and solution, coupled with advocacy during windows of opportunity, contributed to this outcome. The document also discusses the role of biofortification champions, the importance of advocacy, and the need for continued support and funding to sustain and scale biofortification efforts in Africa. The report concludes with recommendations for future actions, emphasizing the importance of national government funding and the integration of biofortification into national agricultural plans.</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Mainstreaming of biofortification in the African Union: Evaluation of CGIAR contributions to a policy outcome trajectory</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1211,35 +1588,65 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>WHEAT, INRA Morocco</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>Morocco</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Morocco, seed system, varietal turn-over, certified seed, INRA</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>&lt;Not Defined&gt;</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>2013-2019</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>"Environmental health and biodiversity; Poverty reduction, livelihoods and jobs"</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>Seed System Development and Varietal Turn-over in Morocco</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>The document reports on a qualitative outcome study titled "Morocco’s seed system makes progress, but some challenges still remain," completed in 2020. Commissioned by WHEAT and INRA Morocco, the study is part of the project P1736, which aims to inform R4D strategies through foresight and targeting. The study highlights the progress and challenges within Morocco's seed system, noting that despite significant efforts, varietal turnover remains low, with older varieties still occupying a large portion of the wheat area. However, the seed business has seen the emergence of over 300 new enterprises focusing on regional needs, leading to a shift towards non-expired plant variety protection (PVP) European varieties and enabling significant varietal turnover. The "Boudour" project invested US$45 million in certified seed sales, although INRA-CGIAR derived varieties have lost market share. The study is linked to the CGIAR Strategic Results Framework, aiming to increase the adoption of improved varieties by farm households. The geographic focus of the study is national, specifically in Morocco.</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Morocco’s seed system makes progress, but some challenges still remain</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -1268,35 +1675,65 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>CIMMYT</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>Malawi</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>maize, pigeonpea, cowpea, soybeans, legume, Zea mays L., Vigna unguiculata L., Cajanus cajan L.</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Farming systems, Climate-smart agriculture, Southern Africa, No-tillage, Malawi</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s13593-020-0608-9</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>The document does not specify a specific period analyzed in terms of start and end dates.</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Cultivation of crops (cereals)</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>"Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs"</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Bridging Disciplinary Gaps in Conservation Agriculture Research in Malawi</t>
-        </is>
-      </c>
       <c r="K14" t="inlineStr">
+        <is>
+          <t>The document does not specify a particular period analyzed in terms of start and end dates.</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Cultivation of crops (maize)</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs; Environmental health and biodiversity</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Bridging Disciplinary Approaches in Conservation Agriculture Research in Malawi</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>The review article discusses the challenges and opportunities in conservation agriculture (CA) research in Malawi, highlighting the need for interdisciplinary approaches to understand what forms of CA work, where, for whom, and why. Despite the biophysical benefits of CA, adoption rates among smallholder farmers in Africa remain low, unlike in countries like Brazil and Argentina. The article identifies two main disciplinary approaches in CA research: agro-ecological and socio-economic, each addressing different aspects of the CA question but failing to fully integrate the 'why' component. The authors argue for the integration of comprehensive datasets, participatory methods, and on-farm trials to bridge the gap between these approaches and better understand the complex interactions within farming systems. They recommend enhancing data compatibility, involving farmers in research design, and using ethnographic methods to capture the dynamic and contextual nature of CA adoption and adaptation. The study emphasizes the importance of interdisciplinary research to address the persistent knowledge gaps and improve CA adoption in diverse socio-economic and agro-ecological contexts.</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Bridging the disciplinary gap in conservation agriculture research, in Malawi. A review</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1310,7 +1747,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ESA</t>
+          <t>Multiple</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1325,35 +1762,65 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>CIMMYT, CIAT, IITA, CIP, IFPRI, HarvestPlus, RTB, A4NH, FARA, AUDA-NEPAD, AUC-DREA, AUC-DSA</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>orange fleshed sweetpotato, rice, wheat, maize, beans, cassava, millet</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>biofortification, African Union, CGIAR, policy change, nutrition</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>10.4160/978929060-5522</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>2014-2020</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>Cultivation of crops (roots and tubers)</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>Nutrition, health and food security; Gender equality, youth and social inclusion</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Mainstreaming of Biofortification in the African Union: Evaluation of CGIAR Contributions to a Policy Outcome Trajectory</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Mainstreaming Biofortification in the African Union: Evaluation of CGIAR Contributions</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>The document evaluates the contributions of CGIAR, particularly the Research Programs on Roots, Tubers and Bananas (RTB) and Agriculture for Nutrition and Health (A4NH), in mainstreaming biofortification within the African Union (AU). It highlights the collaborative efforts of HarvestPlus/A4NH and CIP/RTB in advocating for biofortification as a solution to micronutrient malnutrition, leading to a continental declaration ready to be tabled at an AU Summit. The evaluation uses a policy window theory of change to understand how CGIAR's framing of the problem and solution, coupled with advocacy during windows of opportunity, contributed to this outcome. The document also discusses the role of biofortification champions, the importance of advocacy, and the need for continued support and funding to sustain and scale biofortification efforts in Africa. The evaluation concludes that while internal tensions existed, they did not significantly hinder the process, and emphasizes the importance of integrating gender considerations and leveraging existing AU strategies for future scaling.</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Mainstreaming of biofortification in the African Union: Evaluation of CGIAR contributions to a policy outcome trajectory</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1382,35 +1849,65 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>WLE, CCAFS, SMO</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>India</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>There are no crops mentioned in the text.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Solar-powered irrigation, Climate-smart research, Greenhouse gas emissions, India, CGIAR</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>&lt;Not Defined&gt;</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>2020-2020</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Cultivation of crops (solar-powered irrigation)</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>"Climate adaptation and mitigation; Environmental health and biodiversity"</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Cultivation of crops (fruits and vegetables)</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Climate adaptation and mitigation; Environmental health and biodiversity</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
         <is>
           <t>Solar-Powered Irrigation and Climate-Smart Research in India</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>The document titled "Reporting 2021 Evidences" focuses on Study #4089, which is linked to the project P1751 concerning on and off-grid solar in Africa and Asia. The study is a qualitative outcome evaluation completed in 2020, assessing the impact of climate-smart research on solar-powered irrigation in India. This research was conducted under the auspices of the CGIAR Research Program on Water, Land and Ecosystems (WLE), the CGIAR Research Program on Climate Change, Agriculture and Food Security (CCAFS), and the CGIAR System Management Office (SMO). The study aims to substantiate contributions to policy and includes recommendations and ex-ante modeling. It aligns with the CGIAR Strategic Results Framework, particularly focusing on reducing net greenhouse gas emissions and promoting sustainable agro-ecosystems. The geographic scope of the study is national, specifically targeting India. The report was generated on August 19, 2022.</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Outcome evaluation of climate-smart research on solar-powered irrigation in India conducted under the WLE, CCAFS and SMO</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -1439,35 +1936,66 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>CIP, CIAT, IITA, CIRAD</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>Kenya</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Potato, bananas, plantains, cassava, sweetpotato, yams, minor roots and tubers, maize, Solanum tuberosum, tomato, eggplant, African nightshade, Allium cepa, Allium sativum, Brassica nigra, cereals, legumes</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>seed potato, regulatory frameworks, quality assurance, plant diseases, Kenya</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>10.4160/23096586RTBWP20211</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>2017-2018</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Cultivation of crops (potatoes)</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs; Gender equality, youth and social inclusion</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Cultivation of crops (vegetatively propagated crops)</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>"Poverty reduction, livelihoods and jobs; Nutrition, health and food security; Environmental health and biodiversity"</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
         <is>
           <t>Exploring Regulatory Frameworks for Seed Potato Quality Improvement in Kenya</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>The document explores the regulatory framework for improving the availability, access, and quality of vegetatively propagated crop seed, specifically focusing on potato seed in Kenya. It highlights the challenges faced by the Kenyan potato sector, including a significant shortage of certified seed, which constitutes less than 2% of the seed planted. The study examines the current seed regulatory framework and its implications for seed potato production, emphasizing the need for reforms to accommodate both formal and informal seed systems. The document discusses the divergent perspectives among stakeholders, with some advocating for increased availability of "clean seed" to meet food security objectives, while others emphasize the need for certified seed to prevent the spread of diseases. It also addresses the role of various stakeholders, including government agencies, private companies, and NGOs, in the seed potato value chain and the challenges posed by the current regulatory framework.
+The paper suggests several policy options to improve the seed potato system in Kenya, including recognizing dual production models, creating separate regulations for different seed systems, and supporting integrated seed health strategies. It emphasizes the importance of inclusive stakeholder consultations to identify common interest spaces and negotiate trade-offs between short-term food security and long-term plant health objectives. The document concludes that a holistic approach to seed quality assurance, recognizing the interdependence of different seed systems, is essential for improving the overall plant health system and achieving national development goals.</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Exploring the regulatory space for improving availability, access and quality of vegetatively propagated crop seed: potato in Kenya</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -1496,35 +2024,65 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>International Potato Center</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>Bangladesh</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>orange-fleshed sweetpotato, potato, rice, vegetables, jute, wheat, pulses, tobacco, betel leaf, maize, spices, aromatic crops, sugarcane, mustard seed, sweetpotato leaves, egg, milk, fish, meat, leafy vegetables, red amaranth, aroid leaves, spinach, stem amaranth, kangkong, sponge gourd, lemon, ginger, wood apple, taro</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Community Nutrition Scholars, Orange-fleshed sweetpotato, Child nutrition, Homestead gardening, Behavior change</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>10.4160/9789290605683</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>2018-2020</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>Cultivation of crops (sweetpotato and potato)</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Nutrition, health and food security; Gender equality, youth and social inclusion; Poverty reduction, livelihoods and jobs</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Contribution of Community Nutrition Scholars and Utilization of Orange-Fleshed Sweetpotato in Child Nutrition and Health in Southern Bangladesh.</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs; Gender equality, youth and social inclusion</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Contribution of Community Nutrition Scholars to Child Nutrition and Health in Southern Bangladesh</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>The document is a comprehensive assessment of a project aimed at improving the nutrition and health of young children in southern Bangladesh through the use of Community Nutrition Scholars (CNS) and the introduction of orange-fleshed sweetpotato (OFSP). Conducted by the International Potato Center, the study evaluates the impact of CNS-led training sessions on mothers, focusing on changes in child feeding practices, food preparation, and hygiene. The findings indicate significant behavior changes among women and their families, with improved child nutrition and health practices, increased consumption of OFSP, and greater empowerment of women. The study also highlights the challenges faced, such as initial community resistance and the potential burden of additional responsibilities on women. The assessment suggests that the project has been successful in scaling new practices, with an estimated 50,000 households benefiting from the knowledge shared by the 5,000 women trained. The document concludes with recommendations for sustaining these changes, emphasizing the need for continued support and involvement of family members to ensure the long-term success of the interventions.</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Toward more nutritious diets for young children in southern Bangladesh</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1553,35 +2111,65 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>CIMMYT, ICARDA, ICRISAT, CIAT, IRRI, CIP, IFPRI, CCAFS, Excellence in Breeding Platform, Crops to End Hunger Initiative</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>wheat, sorghum, pearl millet, groundnut, chickpea, rice, maize, barley, cassava, potato, sweet potato, common bean, lentil</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>crop modeling, climate change, breeding programs, genotypic adaptation, CGIAR</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/csc2.20048</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>1961-2000</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals and legumes)</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Climate adaptation and mitigation; Nutrition, health and food security</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>"Climate adaptation and mitigation; Nutrition, health and food security"</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
         <is>
           <t>Accelerating Crop Breeding for Climate Change Adaptation Using CGIAR Modeling Approaches</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>The document discusses the role of crop modeling in accelerating crop breeding, particularly within the CGIAR system, to adapt to climate change. It highlights the importance of model-based approaches in assessing genotypic adaptability, characterizing target breeding environments, and predicting breeding values. The document reviews various modeling strategies, including process-based eco-physiological models and statistical approaches, to understand genotype-environment-management interactions. It emphasizes the need for collaboration between modelers and breeding programs to enhance breeding gains, suggesting that crop modelers should be integrated into crop improvement teams. The document also identifies limitations in current modeling approaches and suggests future work, such as developing simpler models, modernizing data storage, and leveraging phenotyping and breeding data for modeling key traits. The ultimate goal is to make crop modeling more effective in contributing to targeted and impactful breeding programs under changing climates.</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>CGIAR modeling approaches for resource-constrained scenarios: I. Accelerating crop breeding for a changing climate</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1610,35 +2198,65 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>CIMMYT, IRRI, IFPRI, ICRISAT, CIP, CIAT, ICARDA, CGIAR Research Program on Policies, Institutions and Markets, CGIAR Research Program on Climate Change, Agriculture, and Food Security, Global Futures and Strategic Foresight, CGIAR Platform for Big Data in Agriculture, Excellence in Breeding Platform</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Maize, Wheat, Rice, Sorghum, Potato, Common Bean, Pigeonpea, Mucuna, Oil Palm, Fish, Roots, Tubers, Banana</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>CGIAR, crop modeling, socioeconomic analysis, bio-economic models, climate change</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/csc2.20114</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>2010-2019</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals, legumes, roots, tubers, and bananas)</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>"Climate adaptation and mitigation; Nutrition, health and food security; Poverty reduction, livelihoods and jobs"</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>CGIAR Modeling Approaches for Socioeconomic Analysis in Resource-Constrained Scenarios</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs; Nutrition, health and food security</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Models for Analyzing Socioeconomic Factors to Improve Policy Recommendations in Resource-Constrained Scenarios</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>The document discusses the integration of crop modeling and socioeconomic analysis within the CGIAR framework to enhance policy recommendations and improve agricultural productivity, especially in resource-constrained scenarios. It highlights the importance of interdisciplinary collaboration across various CGIAR centers to address global challenges such as climate change, food security, and poverty alleviation. The document outlines the use of various models, including the IMPACT model, DREAM, and TOA-MD, to assess the economic impacts of agricultural technologies and policies. It emphasizes the need for strategic foresight and ex-ante impact assessment to guide research priorities and policy decisions. The document also discusses the benefits of modeling collaboration, the use of bio-economic models at different scales, and the opportunities presented by new data sources and technologies to improve the accuracy and applicability of these models in addressing complex agri-food systems challenges.</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>CGIAR modeling approaches for resource-constrained scenarios: II. Models for analyzing socioeconomic factors to improve policy recommendations</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1667,35 +2285,66 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t>CIMMYT</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
           <t>India</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Wheat, Rice</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Climate change adaptation, Conservation agriculture, Ex ante risk coping strategy, Learning from past climate extremes, Turbo happy seeder</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1108/IJCCSM-09-2018-0065</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>2013-2016</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="M21" t="inlineStr">
         <is>
           <t>Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Learning Adaptation to Climate Change through Conservation Agriculture in Haryana, India.</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Learning Adaptation to Climate Change from Past Climate Extremes in Haryana, India</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>The document discusses a study on the adoption of conservation agriculture-based wheat production systems (CAW) in Haryana, India, as a strategy to mitigate climate risks, particularly extreme rainfall during the wheat production season. The study, conducted by Jeetendra Prakash Aryal and colleagues from the International Maize and Wheat Improvement Center (CIMMYT), used data from 184 farmers over three wheat seasons (2013-2016) and employed multivariate logit and Tobit models to analyze the drivers and intensity of CAW adoption. Findings indicate that farmers who experienced CAW's benefits during a year of untimely excess rainfall (2014-2015) continued to practice and expand CAW. The study highlights the importance of learning from past climate extremes and farmer-to-farmer communication in technology adoption. It also identifies barriers such as knowledge gaps and limited access to machinery, suggesting that improved communication of scientific evidence and better institutional support could enhance CAW adoption.
+The study emphasizes the role of CAW in enhancing agricultural resilience to climate variability, reducing greenhouse gas emissions, and preventing air pollution from residue burning. It also notes that CAW has economic benefits and a shorter gestation period due to the availability of machinery on rent. The authors recommend facilitating farmer communication, improving custom hiring services for CAW machinery, revising crop loss compensation policies, and involving the private sector to promote CAW adoption. The study concludes that targeting young farmers and providing training can significantly enhance CAW adoption, and calls for further research to generalize its impacts across different regions in India.</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Learning adaptation to climate change from past climate extremes: Evidence from recent climate extremes in Haryana, India</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1724,35 +2373,65 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
+          <t>CRP WHEAT</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>gender norms, wheat agriculture, women empowerment, patriarchal contexts, agricultural technologies</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>&lt;Not Defined&gt;</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="K22" t="inlineStr">
         <is>
           <t>2020-2020</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="M22" t="inlineStr">
         <is>
           <t>Gender equality, youth and social inclusion; No Secondary Impact Area(s)</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="N22" t="inlineStr">
         <is>
           <t>Gender Norms and Wheat Agriculture in Patriarchal Contexts</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>The document reports on a completed synthesis study from 2020, titled "Collaborative analysis of gender norms and wheat agriculture in patriarchal contexts in Afghanistan, Ethiopia, and Pakistan." This study is part of the CRP WHEAT project and contributes to the P1336 project, which focuses on building a gender and social inclusion portfolio in wheat agri-food systems. The study examines the impact of social norms that traditionally view men as farmers and women as homemakers, despite women being active workers and decision-makers in wheat production. It suggests that changing these perceptions could alter household decision-making dynamics and lead to the adoption of new agricultural technologies. The study is multi-national, covering Ethiopia, Afghanistan, and Pakistan, and links to the CGIAR Strategic Results Framework by aiming to adopt technologies that reduce women's labor and energy expenditure.</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Collaborative analysis of gender norms and wheat agriculture in patriarchal contexts in Afghanistan, Ethiopia and Pakistan</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -1781,35 +2460,65 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t>Agrosavia, CIPAV, The Alliance of Bioversity International and CIAT, CGIAR, International Center for Tropical Agriculture (CIAT), Alexander von Humboldt Institute</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>Colombia</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>forage seeds, grains, soy milk, almond milk, legume seeds, hay, silage</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>resilience, food system, sustainable intensification, consumer behavior, traceability</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>hdl.handle.net/10568/108354</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>2020-2020</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>Rearing of livestock (cattle) for food</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>"Nutrition, health and food security; Climate adaptation and mitigation; Gender equality, youth and social inclusion"</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>COVID-19 Impacts and Mitigation in Colombian Bovine Livestock Sector</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs; Climate adaptation and mitigation; Gender equality, youth and social inclusion</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>COVID-19 Impacts and Mitigation in the Colombian Bovine Livestock Sector</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>The document titled "COVID-19 and the bovine livestock sector in Colombia: Current and potential developments, impacts and mitigation options" explores the multifaceted impacts of the COVID-19 pandemic on Colombia's bovine livestock sector. It highlights the negative effects on beef and dairy value chains, including disruptions in production, distribution, and consumption patterns. The crisis has led to increased consumer demand for food safety and traceability, pushing value chains towards more formality and sustainability. The document also discusses the challenges faced by producers, such as increased input prices, labor shortages, and limited access to credit and technical assistance. It emphasizes the importance of digitalization and virtualization in maintaining sector efficiency and suggests potential mitigation strategies to support the sector's recovery and resilience. The study underscores the need for research to understand the full impact of the crisis and to develop long-term solutions for building resilient food systems.</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>COVID-19 and the bovine livestock sector in Colombia: Current and potential developments, impacts and mitigation options</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1838,35 +2547,66 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
+          <t>CIMMYT</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>maize, wheat, rice, soybean, sunflower, sugar beet, cotton, fruit-tree crops, barley, alfalfa</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Remote sensing, Agricultural practices, Impact evaluation, Developing countries, Satellite data</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s13593-020-0610-2</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>1972-2018</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>"Environmental health and biodiversity; Climate adaptation and mitigation"</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>Use of Satellite Data in Estimating Adoption and Impacts of Agricultural Practices in Developing Countries</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Environmental health and biodiversity; Climate adaptation and mitigation</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Use of Satellite Data in Evaluating Adoption and Impact of Agricultural Practices in Developing Countries</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>The document is a scoping review that examines the use of satellite data to estimate the adoption and impacts of agricultural management practices in developing countries. It highlights the limitations of conventional evaluation methods that rely on farm-household surveys, which are often costly and prone to errors. The review covers 54 studies that utilize satellite data to assess agricultural practices such as cropping intensity, tillage, crop residue cover, irrigation, and soil and water conservation. The findings suggest that satellite data can effectively detect these practices and provide timely, accurate information over large geographic areas. However, the review notes that few studies have explored the economic impacts of these practices, and more interdisciplinary research is needed to integrate satellite data into research-for-development evaluations.
+The document also discusses the potential of satellite data to improve yield estimation and measure environmental and economic outcomes. It emphasizes the advantages of satellite data, such as providing long-term, large-scale observations that can complement traditional survey data. The review identifies challenges in using satellite data, including the need for high-resolution imagery and the integration of socioeconomic variables. It concludes that while satellite data offer significant potential for enhancing agricultural research, there is a need for better integration with conventional methods and more collaboration between remote sensing and economic researchers.</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Estimating adoption and impacts of agricultural management practices in developing countries using satellite data. A scoping review</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1895,35 +2635,65 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
+          <t>CIAT, Alliance of Bioversity International and CIAT, ICRISAT, International Research Institute for Climate and Society</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>crops, mixed farming systems, commodity crops</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Climate services, climate risk, institutional learning, impact pathway, theory of change</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>https://ccafs.cgiar.org/donors</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>2017-2022</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Cultivation of crops (cereals)</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Cultivation of crops (cereals, legumes, fruits, and vegetables)</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Lessons learnt in CCAFS Flagship 4 Phase II: Climate Services and Safety Nets in Agriculture</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Lessons Learnt in Climate Services and Safety Nets in Agriculture</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>The document is a working paper by Lorna Born, titled "Lessons learnt in CCAFS Flagship 4 Phase II," which is part of the CGIAR Research Program on Climate Change, Agriculture and Food Security (CCAFS). The paper reviews the work conducted under Flagship Program 4, focusing on Climate Services and Safety Nets in Latin America, Asia, and Africa. It aims to document challenges, opportunities, and lessons learned over the past five years of research and implementation. The review highlights the importance of using varied metrics to measure impact, understanding the context of interventions, and evaluating how climate information is used in decision-making. It also emphasizes the need for adaptive management, effective communication of forecast uncertainty, and the sustainability of climate services efforts beyond project timelines. The paper underscores the role of south-south knowledge exchange and the challenges of balancing scientific advancement with development impacts in agricultural research-for-development projects.</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Lessons learnt in CCAFS Flagship 4 Phase II</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -1947,40 +2717,66 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Ex post impact study/impact assesment</t>
+          <t>Outcome studies</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
+          <t>ILRI</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
           <t>Rwanda</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Girinka, nutrition, livestock, Rwanda, food security</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>https://cgspace.cgiar.org/handle/10568/114623</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>2020-2020</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>Rearing of livestock (cattle) for food</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="M26" t="inlineStr">
         <is>
           <t>Nutrition, health and food security; Poverty reduction, livelihoods and jobs</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Impact of Livestock Asset Transfer on Nutrition and Food Security</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Impact of Girinka program on nutrition and food security in Rwanda</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>The document reports on a study titled "Impact of Girinka program on child nutritional status and household food security," which is part of the 2021 evidences under study #4085. The study, commissioned by ILRI, is linked to the project P1680, focusing on nutrition-sensitive livestock interventions. It examines the impact of the Girinka program, a livestock asset transfer initiative by the Government of Rwanda and partners, including ILRI, aimed at improving incomes, nutrition, soil fertility, and social integration since 2006. The study compares nutrition outcomes between households participating in the Girinka program and those eligible but not yet participating. Although the results are not yet published in a peer-reviewed journal, a brief is available. The study is national in scope, focusing on Rwanda, and contributes to the CGIAR system level reporting, particularly in increasing access to diverse nutrient-rich foods.</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Impact of Girinka program on child nutritional status and household food security</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -2009,35 +2805,66 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
+          <t>CIMMYT, CCAFS</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>maize, rice, wheat, soybean, sorghum, pigeon pea, soybean, wheat, red grams, mung bean, peanuts, millet, jute, potato, cotton, barley</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Climate change, Adaptation, South Asia, Agriculture, Smallholder production systems</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s10668-019-00414-4</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>1980-2014</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs; Nutrition, health and food security</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
         <is>
           <t>Climate Change Adaptation in South Asian Agriculture: CGIAR's Role in Enhancing Resilience and Sustainability</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>The document discusses the vulnerability of agriculture in South Asia to climate change and the necessity for adaptation measures to sustain productivity and enhance resilience. It reviews the impacts of climate change on crop production, highlighting that climatic variability accounts for a significant portion of yield variability. The document emphasizes the importance of institutional change, funding, and dynamic policies for long-term adaptation, rather than solely focusing on agricultural technology. It outlines various adaptation options, including soil management, crop diversification, water management, and sustainable land management, and discusses the role of risk management strategies like crop insurance and community-based adaptation. The document also highlights the need for international cooperation and integrated agro-meteorological advisory services to support adaptation efforts.
+Furthermore, the document examines the challenges and future prospects of climate change adaptation in South Asian agriculture, emphasizing the importance of enabling policy and institutional mechanisms. It notes that while national-level policies have been devised, their financing and implementation remain critical issues. The document calls for improved understanding of farmer adaptation behavior and stresses the need for coordination at different institutional levels. It concludes that despite the availability of adaptation options, inefficient institutions and financing could hinder the region's ability to tackle future climate challenges, and it identifies areas for further research, particularly in assessing the impact of climate variables other than temperature on crop yields.</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Climate change and agriculture in South Asia: adaptation options in smallholder production systems</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
@@ -2066,35 +2893,65 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
+          <t>CIAT, ILRI, ICRAF, CIMMYT, IITA</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
           <t>Kenya</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>"Increase in household welfare; per capita household expenditure; 1,298"</t>
-        </is>
-      </c>
       <c r="G28" t="inlineStr">
         <is>
+          <t>maize, beans, potatoes, peas, sorghum, sweet potatoes, cassava</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Agriculture, climate change, food security, climate-smart agriculture, impact assessment</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>https://ccafs.cgiar.org/donors</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Increase in household welfare; Ksh; 444 to 779</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
           <t>2011-2020</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Cultivation of crops (cereals, legumes, fruits, and vegetables) and Rearing of livestock (cattle) for food.</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>"Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs; Nutrition, health and food security"</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Impact of CCAFS Engagement on Climate-Smart Agriculture Adoption in Kenya</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>"Cultivation of crops (cereals, legumes, fruits, and vegetables)"</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Climate adaptation and mitigation; Poverty reduction, livelihoods and jobs; Nutrition, health and food security</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>CCAFS Impact on Climate-Smart Agriculture Adoption in Kenya</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>The report assesses the impact of the CGIAR Research Program on Climate Change, Agriculture and Food Security (CCAFS) on national policy engagement in Kenya, focusing on the uptake of climate-smart agriculture (CSA) technologies and practices. Conducted in December 2020 by Boscow Okumu, the study evaluates the influence of CCAFS interventions at both policy and household levels, using a mix of qualitative and quantitative methods. The findings indicate that CCAFS has significantly contributed to the development of policies promoting CSA, although coordination between national and county governments remains weak. At the household level, factors such as age, education, and smartphone ownership influence the adoption of CSA practices, which have been shown to improve agricultural yield, livestock holding, and household welfare. The report highlights the need for better coordination and tailored interventions to enhance the adoption of CSA practices and improve food security and resilience among smallholder farmers in Kenya.</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>CCAFS impact assessment of national policy engagement in Kenya on uptake of climate-smart agriculture technologies and practices</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -2123,35 +2980,65 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
+          <t>HarvestPlus</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
           <t>Bangladesh</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>zinc rice, consumer acceptance, biofortification, Bangladesh, nutritional information</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>&lt;Not Defined&gt;</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>2020-2020</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>Cultivation of crops (cereals)</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="M29" t="inlineStr">
         <is>
           <t>Nutrition, health and food security; No Secondary Impact Area(s)</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="N29" t="inlineStr">
         <is>
           <t>Consumer Acceptance and Demand for Zinc Biofortified Rice in Bangladesh</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>The document reports on a study conducted in 2020, titled "Consumer acceptance study for zinc rice in Bangladesh," commissioned by HarvestPlus. The study, part of the project P335 under Study #3039, aimed to assess consumer acceptance and demand for low-milled and biofortified rice, particularly focusing on zinc rice. It explored whether providing nutritional information about zinc's benefits and availability in biofortified and low-milled rice would influence consumer acceptance and demand. The findings indicated that Bangladeshi consumers are willing to pay a 4-5% premium for these nutritional strategies if adequately informed. Among the strategies, high zinc rice was identified as the optimal approach to address zinc deficiency. The study's results are yet to be published, and it contributes to the CGIAR's strategic goal of increasing the availability of diverse nutrient-rich foods. The geographic scope of the study is national, focusing on Bangladesh.</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Consumer acceptance study for zinc rice in Bangladesh</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -2180,35 +3067,61 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
+          <t>ILRI</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
           <t>Ethiopia</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Community Conversations, gender transformational, small ruminant production, Ethiopia, ILRI innovation</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>&lt;Not Defined&gt;</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
         <is>
           <t>Not reported; NA; NA</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="K30" t="inlineStr">
         <is>
           <t>2020-2020</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="L30" t="inlineStr">
         <is>
           <t>Rearing of livestock (small ruminants) for food</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="M30" t="inlineStr">
         <is>
           <t>Gender equality, youth and social inclusion; Poverty reduction, livelihoods and jobs</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="N30" t="inlineStr">
         <is>
           <t>Gender Transformational Approaches in Small Ruminant Production in Ethiopia</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>The document titled "Reporting 2021 Evidences" focuses on Study #3532, which is part of the project P607 - Activity 2.2.1, aimed at developing and evaluating herd health packages. The study, completed in 2020, assesses the impact of Community Conversations as a gender transformational approach in small ruminant production in Ethiopia. This approach, an innovation by ILRI, is analyzed through change stories and reflections from community members and partners, as well as surveys conducted before and after the community conversations. The study aligns with the CGIAR Strategic Results Framework, particularly in promoting gender-equitable control of productive assets, enhancing women's and young people's decision-making capacities, and closing yield gaps through improved practices. The geographic scope of the study is national, focusing specifically on Ethiopia. The document does not provide specific comments or links to MELIA publications.</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Impact of Community Conversations as a gender transformational approach in small ruminant production in Ethiopia</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
         <is>
           <t>2022</t>
         </is>

</xml_diff>